<commit_message>
clean files:parameterized original census files and modified census files locations
</commit_message>
<xml_diff>
--- a/main_census_merge/reference_data_files/Census_Variables.xlsx
+++ b/main_census_merge/reference_data_files/Census_Variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\Criminal_Justice\Projects\main_census_merge\reference_data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salma/Studies/Research/Criminal_Justice/research_projects/main_census_merge/reference_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E884DB6-8ACA-3745-8F66-1C8DD7A6C5D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="9495" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="283">
   <si>
     <t>GEO.id</t>
   </si>
@@ -865,13 +866,22 @@
   </si>
   <si>
     <t>P12D049</t>
+  </si>
+  <si>
+    <t>NEW VARIABLES</t>
+  </si>
+  <si>
+    <t>First col headers</t>
+  </si>
+  <si>
+    <t>Second col headers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -892,8 +902,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -912,6 +936,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -925,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -936,6 +966,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1215,28 +1254,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C16386"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="4">
         <v>2000</v>
       </c>
@@ -1252,7 +1291,7 @@
       <c r="L2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1292,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1351,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1371,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1392,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1373,7 +1412,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1393,7 +1432,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1413,7 +1452,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1433,7 +1472,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1492,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1473,7 +1512,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1493,7 +1532,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1513,7 +1552,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1533,7 +1572,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1553,7 +1592,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1573,7 +1612,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1593,7 +1632,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1613,7 +1652,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +1672,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1692,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1673,7 +1712,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1693,7 +1732,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1713,7 +1752,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1733,7 +1772,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1753,7 +1792,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1773,7 +1812,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1793,7 +1832,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1813,7 +1852,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1833,7 +1872,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1892,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1912,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1893,7 +1932,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1913,7 +1952,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1933,7 +1972,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1953,7 +1992,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1973,7 +2012,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1993,7 +2032,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2013,7 +2052,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -2033,7 +2072,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2053,7 +2092,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2073,7 +2112,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2093,7 +2132,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2113,7 +2152,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2133,7 +2172,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2153,7 +2192,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2173,7 +2212,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2193,7 +2232,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2213,7 +2252,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2233,7 +2272,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2253,7 +2292,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2273,7 +2312,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2300,1166 +2339,1273 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K16386"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.5" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="4">
         <v>2000</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="4">
+      <c r="D2" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H2" s="4">
         <v>2010</v>
       </c>
+      <c r="J2" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="K2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="H3" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I4" t="s">
         <v>52</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="K4" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I5" t="s">
         <v>53</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H6" t="s">
         <v>2</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I6" t="s">
         <v>54</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="K6" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>182</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H7" t="s">
         <v>104</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J7" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="K7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H8" t="s">
         <v>105</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I8" t="s">
         <v>56</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J8" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="K8" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H9" t="s">
         <v>106</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I9" t="s">
         <v>57</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="K9" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H10" t="s">
         <v>107</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I10" t="s">
         <v>58</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J10" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="K10" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>186</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H11" t="s">
         <v>108</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I11" t="s">
         <v>59</v>
       </c>
-      <c r="K10" t="s">
+      <c r="J11" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="K11" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H12" t="s">
         <v>109</v>
       </c>
-      <c r="J11" t="s">
+      <c r="I12" t="s">
         <v>60</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J12" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="K12" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H13" t="s">
         <v>110</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I13" t="s">
         <v>61</v>
       </c>
-      <c r="K12" t="s">
+      <c r="J13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="K13" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>189</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H14" t="s">
         <v>111</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I14" t="s">
         <v>62</v>
       </c>
-      <c r="K13" t="s">
+      <c r="J14" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="K14" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>190</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H15" t="s">
         <v>112</v>
       </c>
-      <c r="J14" t="s">
+      <c r="I15" t="s">
         <v>63</v>
       </c>
-      <c r="K14" t="s">
+      <c r="J15" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="K15" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>191</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H16" t="s">
         <v>113</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I16" t="s">
         <v>64</v>
       </c>
-      <c r="K15" t="s">
+      <c r="J16" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="K16" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>192</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H17" t="s">
         <v>114</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I17" t="s">
         <v>65</v>
       </c>
-      <c r="K16" t="s">
+      <c r="J17" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="K17" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>193</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H18" t="s">
         <v>115</v>
       </c>
-      <c r="J17" t="s">
+      <c r="I18" t="s">
         <v>66</v>
       </c>
-      <c r="K17" t="s">
+      <c r="J18" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="K18" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>194</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H19" t="s">
         <v>116</v>
       </c>
-      <c r="J18" t="s">
+      <c r="I19" t="s">
         <v>67</v>
       </c>
-      <c r="K18" t="s">
+      <c r="J19" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="K19" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H20" t="s">
         <v>117</v>
       </c>
-      <c r="J19" t="s">
+      <c r="I20" t="s">
         <v>68</v>
       </c>
-      <c r="K19" t="s">
+      <c r="J20" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="K20" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H21" t="s">
         <v>118</v>
       </c>
-      <c r="J20" t="s">
+      <c r="I21" t="s">
         <v>69</v>
       </c>
-      <c r="K20" t="s">
+      <c r="J21" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="K21" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H22" t="s">
         <v>119</v>
       </c>
-      <c r="J21" t="s">
+      <c r="I22" t="s">
         <v>70</v>
       </c>
-      <c r="K21" t="s">
+      <c r="J22" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="K22" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H23" t="s">
         <v>120</v>
       </c>
-      <c r="J22" t="s">
+      <c r="I23" t="s">
         <v>71</v>
       </c>
-      <c r="K22" t="s">
+      <c r="J23" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="K23" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>199</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H24" t="s">
         <v>121</v>
       </c>
-      <c r="J23" t="s">
+      <c r="I24" t="s">
         <v>72</v>
       </c>
-      <c r="K23" t="s">
+      <c r="J24" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="K24" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>200</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I24" t="s">
+      <c r="H25" t="s">
         <v>122</v>
       </c>
-      <c r="J24" t="s">
+      <c r="I25" t="s">
         <v>73</v>
       </c>
-      <c r="K24" t="s">
+      <c r="J25" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="K25" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>201</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="I25" t="s">
+      <c r="H26" t="s">
         <v>123</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I26" t="s">
         <v>74</v>
       </c>
-      <c r="K25" t="s">
+      <c r="J26" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="K26" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>202</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="I26" t="s">
+      <c r="H27" t="s">
         <v>124</v>
       </c>
-      <c r="J26" t="s">
+      <c r="I27" t="s">
         <v>75</v>
       </c>
-      <c r="K26" t="s">
+      <c r="J27" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="K27" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>203</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="I27" t="s">
+      <c r="H28" t="s">
         <v>125</v>
       </c>
-      <c r="J27" t="s">
+      <c r="I28" t="s">
         <v>76</v>
       </c>
-      <c r="K27" t="s">
+      <c r="J28" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="K28" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I28" t="s">
+      <c r="H29" t="s">
         <v>126</v>
       </c>
-      <c r="J28" t="s">
+      <c r="I29" t="s">
         <v>77</v>
       </c>
-      <c r="K28" t="s">
+      <c r="J29" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="K29" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>205</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="I29" t="s">
+      <c r="H30" t="s">
         <v>127</v>
       </c>
-      <c r="J29" t="s">
+      <c r="I30" t="s">
         <v>78</v>
       </c>
-      <c r="K29" t="s">
+      <c r="J30" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="K30" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>79</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>206</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="I30" t="s">
+      <c r="H31" t="s">
         <v>128</v>
       </c>
-      <c r="J30" t="s">
+      <c r="I31" t="s">
         <v>79</v>
       </c>
-      <c r="K30" t="s">
+      <c r="J31" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="K31" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>207</v>
       </c>
-      <c r="I31" t="s">
+      <c r="H32" t="s">
         <v>129</v>
       </c>
-      <c r="J31" t="s">
+      <c r="I32" t="s">
         <v>80</v>
       </c>
-      <c r="K31" t="s">
+      <c r="J32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>208</v>
       </c>
-      <c r="I32" t="s">
+      <c r="H33" t="s">
         <v>130</v>
       </c>
-      <c r="J32" t="s">
+      <c r="I33" t="s">
         <v>81</v>
       </c>
-      <c r="K32" t="s">
+      <c r="J33" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>209</v>
       </c>
-      <c r="I33" t="s">
+      <c r="H34" t="s">
         <v>131</v>
       </c>
-      <c r="J33" t="s">
+      <c r="I34" t="s">
         <v>82</v>
       </c>
-      <c r="K33" t="s">
+      <c r="J34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>83</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>210</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H35" t="s">
         <v>132</v>
       </c>
-      <c r="J34" t="s">
+      <c r="I35" t="s">
         <v>83</v>
       </c>
-      <c r="K34" t="s">
+      <c r="J35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>84</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>211</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H36" t="s">
         <v>133</v>
       </c>
-      <c r="J35" t="s">
+      <c r="I36" t="s">
         <v>84</v>
       </c>
-      <c r="K35" t="s">
+      <c r="J36" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>85</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>212</v>
       </c>
-      <c r="I36" t="s">
+      <c r="H37" t="s">
         <v>134</v>
       </c>
-      <c r="J36" t="s">
+      <c r="I37" t="s">
         <v>85</v>
       </c>
-      <c r="K36" t="s">
+      <c r="J37" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>213</v>
       </c>
-      <c r="I37" t="s">
+      <c r="H38" t="s">
         <v>135</v>
       </c>
-      <c r="J37" t="s">
+      <c r="I38" t="s">
         <v>86</v>
       </c>
-      <c r="K37" t="s">
+      <c r="J38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>87</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>214</v>
       </c>
-      <c r="I38" t="s">
+      <c r="H39" t="s">
         <v>136</v>
       </c>
-      <c r="J38" t="s">
+      <c r="I39" t="s">
         <v>87</v>
       </c>
-      <c r="K38" t="s">
+      <c r="J39" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>215</v>
       </c>
-      <c r="I39" t="s">
+      <c r="H40" t="s">
         <v>137</v>
       </c>
-      <c r="J39" t="s">
+      <c r="I40" t="s">
         <v>88</v>
       </c>
-      <c r="K39" t="s">
+      <c r="J40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>89</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>216</v>
       </c>
-      <c r="I40" t="s">
+      <c r="H41" t="s">
         <v>138</v>
       </c>
-      <c r="J40" t="s">
+      <c r="I41" t="s">
         <v>89</v>
       </c>
-      <c r="K40" t="s">
+      <c r="J41" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>217</v>
       </c>
-      <c r="I41" t="s">
+      <c r="H42" t="s">
         <v>139</v>
       </c>
-      <c r="J41" t="s">
+      <c r="I42" t="s">
         <v>90</v>
       </c>
-      <c r="K41" t="s">
+      <c r="J42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>218</v>
       </c>
-      <c r="I42" t="s">
+      <c r="H43" t="s">
         <v>140</v>
       </c>
-      <c r="J42" t="s">
+      <c r="I43" t="s">
         <v>91</v>
       </c>
-      <c r="K42" t="s">
+      <c r="J43" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>92</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>219</v>
       </c>
-      <c r="I43" t="s">
+      <c r="H44" t="s">
         <v>141</v>
       </c>
-      <c r="J43" t="s">
+      <c r="I44" t="s">
         <v>92</v>
       </c>
-      <c r="K43" t="s">
+      <c r="J44" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>93</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>220</v>
       </c>
-      <c r="I44" t="s">
+      <c r="H45" t="s">
         <v>142</v>
       </c>
-      <c r="J44" t="s">
+      <c r="I45" t="s">
         <v>93</v>
       </c>
-      <c r="K44" t="s">
+      <c r="J45" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>221</v>
       </c>
-      <c r="I45" t="s">
+      <c r="H46" t="s">
         <v>143</v>
       </c>
-      <c r="J45" t="s">
+      <c r="I46" t="s">
         <v>94</v>
       </c>
-      <c r="K45" t="s">
+      <c r="J46" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>95</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>222</v>
       </c>
-      <c r="I46" t="s">
+      <c r="H47" t="s">
         <v>144</v>
       </c>
-      <c r="J46" t="s">
+      <c r="I47" t="s">
         <v>95</v>
       </c>
-      <c r="K46" t="s">
+      <c r="J47" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:10">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>96</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>223</v>
       </c>
-      <c r="I47" t="s">
+      <c r="H48" t="s">
         <v>145</v>
       </c>
-      <c r="J47" t="s">
+      <c r="I48" t="s">
         <v>96</v>
       </c>
-      <c r="K47" t="s">
+      <c r="J48" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>224</v>
       </c>
-      <c r="I48" t="s">
+      <c r="H49" t="s">
         <v>146</v>
       </c>
-      <c r="J48" t="s">
+      <c r="I49" t="s">
         <v>97</v>
       </c>
-      <c r="K48" t="s">
+      <c r="J49" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>225</v>
       </c>
-      <c r="I49" t="s">
+      <c r="H50" t="s">
         <v>147</v>
       </c>
-      <c r="J49" t="s">
+      <c r="I50" t="s">
         <v>98</v>
       </c>
-      <c r="K49" t="s">
+      <c r="J50" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>99</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>226</v>
       </c>
-      <c r="I50" t="s">
+      <c r="H51" t="s">
         <v>148</v>
       </c>
-      <c r="J50" t="s">
+      <c r="I51" t="s">
         <v>99</v>
       </c>
-      <c r="K50" t="s">
+      <c r="J51" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>100</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>227</v>
       </c>
-      <c r="I51" t="s">
+      <c r="H52" t="s">
         <v>149</v>
       </c>
-      <c r="J51" t="s">
+      <c r="I52" t="s">
         <v>100</v>
       </c>
-      <c r="K51" t="s">
+      <c r="J52" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>101</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>228</v>
       </c>
-      <c r="I52" t="s">
+      <c r="H53" t="s">
         <v>150</v>
       </c>
-      <c r="J52" t="s">
+      <c r="I53" t="s">
         <v>101</v>
       </c>
-      <c r="K52" t="s">
+      <c r="J53" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
         <v>50</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>229</v>
       </c>
-      <c r="I53" t="s">
+      <c r="H54" t="s">
         <v>151</v>
       </c>
-      <c r="J53" t="s">
+      <c r="I54" t="s">
         <v>102</v>
       </c>
-      <c r="K53" t="s">
+      <c r="J54" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
         <v>51</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>103</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>230</v>
       </c>
-      <c r="I54" t="s">
+      <c r="H55" t="s">
         <v>152</v>
       </c>
-      <c r="J54" t="s">
+      <c r="I55" t="s">
         <v>103</v>
       </c>
-      <c r="K54" t="s">
+      <c r="J55" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wip for creating reqd fips cols. added code for generating fips cnty,place,state cols. working on reindexing cols
</commit_message>
<xml_diff>
--- a/main_census_merge/reference_data_files/Census_Variables.xlsx
+++ b/main_census_merge/reference_data_files/Census_Variables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salma/Studies/Research/Criminal_Justice/research_projects/main_census_merge/reference_data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshaik2\PycharmProjects\projects\research-projects\main_census_merge\reference_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E884DB6-8ACA-3745-8F66-1C8DD7A6C5D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="284">
   <si>
     <t>GEO.id</t>
   </si>
@@ -874,14 +873,17 @@
     <t>First col headers</t>
   </si>
   <si>
-    <t>Second col headers</t>
+    <t>Second col headers - Removed</t>
+  </si>
+  <si>
+    <t>Second col headers-Removed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,12 +908,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -958,7 +961,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -971,9 +973,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1254,1081 +1255,1274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C16386"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="17.5" customWidth="1"/>
-    <col min="16" max="16" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>2000</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="4">
+      <c r="D2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" s="3">
         <v>2010</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>153</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="L2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="G4" t="s">
         <v>52</v>
       </c>
-      <c r="K3" t="s">
+      <c r="H4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="G5" t="s">
         <v>53</v>
       </c>
-      <c r="K4" t="s">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
+      <c r="I5" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>156</v>
       </c>
-      <c r="I5" t="s">
+      <c r="D6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="J5" t="s">
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="K5" t="s">
+      <c r="H6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
+      <c r="I6" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>182</v>
       </c>
-      <c r="I6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" t="s">
         <v>104</v>
       </c>
-      <c r="J6" t="s">
+      <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="K6" t="s">
+      <c r="H7" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
+      <c r="I7" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="I7" t="s">
+      <c r="D8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" t="s">
         <v>105</v>
       </c>
-      <c r="J7" t="s">
+      <c r="G8" t="s">
         <v>56</v>
       </c>
-      <c r="K7" t="s">
+      <c r="H8" t="s">
         <v>232</v>
       </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
+      <c r="I8" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>184</v>
       </c>
-      <c r="I8" t="s">
+      <c r="D9" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" t="s">
         <v>106</v>
       </c>
-      <c r="J8" t="s">
+      <c r="G9" t="s">
         <v>57</v>
       </c>
-      <c r="K8" t="s">
+      <c r="H9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
+      <c r="I9" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>185</v>
       </c>
-      <c r="I9" t="s">
+      <c r="D10" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" t="s">
         <v>107</v>
       </c>
-      <c r="J9" t="s">
+      <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="K9" t="s">
+      <c r="H10" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
+      <c r="I10" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>186</v>
       </c>
-      <c r="I10" t="s">
+      <c r="D11" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" t="s">
         <v>108</v>
       </c>
-      <c r="J10" t="s">
+      <c r="G11" t="s">
         <v>59</v>
       </c>
-      <c r="K10" t="s">
+      <c r="H11" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
+      <c r="I11" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>187</v>
       </c>
-      <c r="I11" t="s">
+      <c r="D12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" t="s">
         <v>109</v>
       </c>
-      <c r="J11" t="s">
+      <c r="G12" t="s">
         <v>60</v>
       </c>
-      <c r="K11" t="s">
+      <c r="H12" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
+      <c r="I12" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>188</v>
       </c>
-      <c r="I12" t="s">
+      <c r="D13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" t="s">
         <v>110</v>
       </c>
-      <c r="J12" t="s">
+      <c r="G13" t="s">
         <v>61</v>
       </c>
-      <c r="K12" t="s">
+      <c r="H13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
+      <c r="I13" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>189</v>
       </c>
-      <c r="I13" t="s">
+      <c r="D14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" t="s">
         <v>111</v>
       </c>
-      <c r="J13" t="s">
+      <c r="G14" t="s">
         <v>62</v>
       </c>
-      <c r="K13" t="s">
+      <c r="H14" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
+      <c r="I14" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>190</v>
       </c>
-      <c r="I14" t="s">
+      <c r="D15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" t="s">
         <v>112</v>
       </c>
-      <c r="J14" t="s">
+      <c r="G15" t="s">
         <v>63</v>
       </c>
-      <c r="K14" t="s">
+      <c r="H15" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" t="s">
+      <c r="I15" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>191</v>
       </c>
-      <c r="I15" t="s">
+      <c r="D16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" t="s">
         <v>113</v>
       </c>
-      <c r="J15" t="s">
+      <c r="G16" t="s">
         <v>64</v>
       </c>
-      <c r="K15" t="s">
+      <c r="H16" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" t="s">
+      <c r="I16" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>192</v>
       </c>
-      <c r="I16" t="s">
+      <c r="D17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" t="s">
         <v>114</v>
       </c>
-      <c r="J16" t="s">
+      <c r="G17" t="s">
         <v>65</v>
       </c>
-      <c r="K16" t="s">
+      <c r="H17" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
+      <c r="I17" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>193</v>
       </c>
-      <c r="I17" t="s">
+      <c r="D18" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" t="s">
         <v>115</v>
       </c>
-      <c r="J17" t="s">
+      <c r="G18" t="s">
         <v>66</v>
       </c>
-      <c r="K17" t="s">
+      <c r="H18" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
+      <c r="I18" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>194</v>
       </c>
-      <c r="I18" t="s">
+      <c r="D19" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" t="s">
         <v>116</v>
       </c>
-      <c r="J18" t="s">
+      <c r="G19" t="s">
         <v>67</v>
       </c>
-      <c r="K18" t="s">
+      <c r="H19" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
+      <c r="I19" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>195</v>
       </c>
-      <c r="I19" t="s">
+      <c r="D20" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" t="s">
         <v>117</v>
       </c>
-      <c r="J19" t="s">
+      <c r="G20" t="s">
         <v>68</v>
       </c>
-      <c r="K19" t="s">
+      <c r="H20" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
+      <c r="I20" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>196</v>
       </c>
-      <c r="I20" t="s">
+      <c r="D21" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" t="s">
         <v>118</v>
       </c>
-      <c r="J20" t="s">
+      <c r="G21" t="s">
         <v>69</v>
       </c>
-      <c r="K20" t="s">
+      <c r="H21" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
+      <c r="I21" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>197</v>
       </c>
-      <c r="I21" t="s">
+      <c r="D22" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" t="s">
         <v>119</v>
       </c>
-      <c r="J21" t="s">
+      <c r="G22" t="s">
         <v>70</v>
       </c>
-      <c r="K21" t="s">
+      <c r="H22" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
+      <c r="I22" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>198</v>
       </c>
-      <c r="I22" t="s">
+      <c r="D23" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" t="s">
         <v>120</v>
       </c>
-      <c r="J22" t="s">
+      <c r="G23" t="s">
         <v>71</v>
       </c>
-      <c r="K22" t="s">
+      <c r="H23" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
+      <c r="I23" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>199</v>
       </c>
-      <c r="I23" t="s">
+      <c r="D24" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" t="s">
         <v>121</v>
       </c>
-      <c r="J23" t="s">
+      <c r="G24" t="s">
         <v>72</v>
       </c>
-      <c r="K23" t="s">
+      <c r="H24" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
+      <c r="I24" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>200</v>
       </c>
-      <c r="I24" t="s">
+      <c r="D25" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" t="s">
         <v>122</v>
       </c>
-      <c r="J24" t="s">
+      <c r="G25" t="s">
         <v>73</v>
       </c>
-      <c r="K24" t="s">
+      <c r="H25" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
+      <c r="I25" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>201</v>
       </c>
-      <c r="I25" t="s">
+      <c r="D26" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" t="s">
         <v>123</v>
       </c>
-      <c r="J25" t="s">
+      <c r="G26" t="s">
         <v>74</v>
       </c>
-      <c r="K25" t="s">
+      <c r="H26" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" t="s">
+      <c r="I26" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>202</v>
       </c>
-      <c r="I26" t="s">
+      <c r="D27" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" t="s">
         <v>124</v>
       </c>
-      <c r="J26" t="s">
+      <c r="G27" t="s">
         <v>75</v>
       </c>
-      <c r="K26" t="s">
+      <c r="H27" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
+      <c r="I27" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>203</v>
       </c>
-      <c r="I27" t="s">
+      <c r="D28" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" t="s">
         <v>125</v>
       </c>
-      <c r="J27" t="s">
+      <c r="G28" t="s">
         <v>76</v>
       </c>
-      <c r="K27" t="s">
+      <c r="H28" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
+      <c r="I28" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>204</v>
       </c>
-      <c r="I28" t="s">
+      <c r="D29" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" t="s">
         <v>126</v>
       </c>
-      <c r="J28" t="s">
+      <c r="G29" t="s">
         <v>77</v>
       </c>
-      <c r="K28" t="s">
+      <c r="H29" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
+      <c r="I29" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>205</v>
       </c>
-      <c r="I29" t="s">
+      <c r="D30" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
         <v>127</v>
       </c>
-      <c r="J29" t="s">
+      <c r="G30" t="s">
         <v>78</v>
       </c>
-      <c r="K29" t="s">
+      <c r="H30" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
+      <c r="I30" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>79</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>206</v>
       </c>
-      <c r="I30" t="s">
+      <c r="D31" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
         <v>128</v>
       </c>
-      <c r="J30" t="s">
+      <c r="G31" t="s">
         <v>79</v>
       </c>
-      <c r="K30" t="s">
+      <c r="H31" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
+      <c r="I31" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>207</v>
       </c>
-      <c r="I31" t="s">
+      <c r="F32" t="s">
         <v>129</v>
       </c>
-      <c r="J31" t="s">
+      <c r="G32" t="s">
         <v>80</v>
       </c>
-      <c r="K31" t="s">
+      <c r="H32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>208</v>
       </c>
-      <c r="I32" t="s">
+      <c r="F33" t="s">
         <v>130</v>
       </c>
-      <c r="J32" t="s">
+      <c r="G33" t="s">
         <v>81</v>
       </c>
-      <c r="K32" t="s">
+      <c r="H33" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>209</v>
       </c>
-      <c r="I33" t="s">
+      <c r="F34" t="s">
         <v>131</v>
       </c>
-      <c r="J33" t="s">
+      <c r="G34" t="s">
         <v>82</v>
       </c>
-      <c r="K33" t="s">
+      <c r="H34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>83</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>210</v>
       </c>
-      <c r="I34" t="s">
+      <c r="F35" t="s">
         <v>132</v>
       </c>
-      <c r="J34" t="s">
+      <c r="G35" t="s">
         <v>83</v>
       </c>
-      <c r="K34" t="s">
+      <c r="H35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>84</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>211</v>
       </c>
-      <c r="I35" t="s">
+      <c r="F36" t="s">
         <v>133</v>
       </c>
-      <c r="J35" t="s">
+      <c r="G36" t="s">
         <v>84</v>
       </c>
-      <c r="K35" t="s">
+      <c r="H36" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>85</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>212</v>
       </c>
-      <c r="I36" t="s">
+      <c r="F37" t="s">
         <v>134</v>
       </c>
-      <c r="J36" t="s">
+      <c r="G37" t="s">
         <v>85</v>
       </c>
-      <c r="K36" t="s">
+      <c r="H37" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>213</v>
       </c>
-      <c r="I37" t="s">
+      <c r="F38" t="s">
         <v>135</v>
       </c>
-      <c r="J37" t="s">
+      <c r="G38" t="s">
         <v>86</v>
       </c>
-      <c r="K37" t="s">
+      <c r="H38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>87</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>214</v>
       </c>
-      <c r="I38" t="s">
+      <c r="F39" t="s">
         <v>136</v>
       </c>
-      <c r="J38" t="s">
+      <c r="G39" t="s">
         <v>87</v>
       </c>
-      <c r="K38" t="s">
+      <c r="H39" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>215</v>
       </c>
-      <c r="I39" t="s">
+      <c r="F40" t="s">
         <v>137</v>
       </c>
-      <c r="J39" t="s">
+      <c r="G40" t="s">
         <v>88</v>
       </c>
-      <c r="K39" t="s">
+      <c r="H40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>89</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>216</v>
       </c>
-      <c r="I40" t="s">
+      <c r="F41" t="s">
         <v>138</v>
       </c>
-      <c r="J40" t="s">
+      <c r="G41" t="s">
         <v>89</v>
       </c>
-      <c r="K40" t="s">
+      <c r="H41" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>90</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>217</v>
       </c>
-      <c r="I41" t="s">
+      <c r="F42" t="s">
         <v>139</v>
       </c>
-      <c r="J41" t="s">
+      <c r="G42" t="s">
         <v>90</v>
       </c>
-      <c r="K41" t="s">
+      <c r="H42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>218</v>
       </c>
-      <c r="I42" t="s">
+      <c r="F43" t="s">
         <v>140</v>
       </c>
-      <c r="J42" t="s">
+      <c r="G43" t="s">
         <v>91</v>
       </c>
-      <c r="K42" t="s">
+      <c r="H43" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>92</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>219</v>
       </c>
-      <c r="I43" t="s">
+      <c r="F44" t="s">
         <v>141</v>
       </c>
-      <c r="J43" t="s">
+      <c r="G44" t="s">
         <v>92</v>
       </c>
-      <c r="K43" t="s">
+      <c r="H44" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>93</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>220</v>
       </c>
-      <c r="I44" t="s">
+      <c r="F45" t="s">
         <v>142</v>
       </c>
-      <c r="J44" t="s">
+      <c r="G45" t="s">
         <v>93</v>
       </c>
-      <c r="K44" t="s">
+      <c r="H45" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
-      <c r="A45" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>221</v>
       </c>
-      <c r="I45" t="s">
+      <c r="F46" t="s">
         <v>143</v>
       </c>
-      <c r="J45" t="s">
+      <c r="G46" t="s">
         <v>94</v>
       </c>
-      <c r="K45" t="s">
+      <c r="H46" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>95</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>222</v>
       </c>
-      <c r="I46" t="s">
+      <c r="F47" t="s">
         <v>144</v>
       </c>
-      <c r="J46" t="s">
+      <c r="G47" t="s">
         <v>95</v>
       </c>
-      <c r="K46" t="s">
+      <c r="H47" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>96</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>223</v>
       </c>
-      <c r="I47" t="s">
+      <c r="F48" t="s">
         <v>145</v>
       </c>
-      <c r="J47" t="s">
+      <c r="G48" t="s">
         <v>96</v>
       </c>
-      <c r="K47" t="s">
+      <c r="H48" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
-      <c r="A48" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>224</v>
       </c>
-      <c r="I48" t="s">
+      <c r="F49" t="s">
         <v>146</v>
       </c>
-      <c r="J48" t="s">
+      <c r="G49" t="s">
         <v>97</v>
       </c>
-      <c r="K48" t="s">
+      <c r="H49" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>225</v>
       </c>
-      <c r="I49" t="s">
+      <c r="F50" t="s">
         <v>147</v>
       </c>
-      <c r="J49" t="s">
+      <c r="G50" t="s">
         <v>98</v>
       </c>
-      <c r="K49" t="s">
+      <c r="H50" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>99</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>226</v>
       </c>
-      <c r="I50" t="s">
+      <c r="F51" t="s">
         <v>148</v>
       </c>
-      <c r="J50" t="s">
+      <c r="G51" t="s">
         <v>99</v>
       </c>
-      <c r="K50" t="s">
+      <c r="H51" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
-      <c r="A51" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>100</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>227</v>
       </c>
-      <c r="I51" t="s">
+      <c r="F52" t="s">
         <v>149</v>
       </c>
-      <c r="J51" t="s">
+      <c r="G52" t="s">
         <v>100</v>
       </c>
-      <c r="K51" t="s">
+      <c r="H52" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
-      <c r="A52" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>101</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>228</v>
       </c>
-      <c r="I52" t="s">
+      <c r="F53" t="s">
         <v>150</v>
       </c>
-      <c r="J52" t="s">
+      <c r="G53" t="s">
         <v>101</v>
       </c>
-      <c r="K52" t="s">
+      <c r="H53" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
-      <c r="A53" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>50</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>229</v>
       </c>
-      <c r="I53" t="s">
+      <c r="F54" t="s">
         <v>151</v>
       </c>
-      <c r="J53" t="s">
+      <c r="G54" t="s">
         <v>102</v>
       </c>
-      <c r="K53" t="s">
+      <c r="H54" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
-      <c r="A54" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>51</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>103</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>230</v>
       </c>
-      <c r="I54" t="s">
+      <c r="F55" t="s">
         <v>152</v>
       </c>
-      <c r="J54" t="s">
+      <c r="G55" t="s">
         <v>103</v>
       </c>
-      <c r="K54" t="s">
+      <c r="H55" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2339,69 +2533,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:M55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22.5" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
-    <col min="14" max="14" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="A2" s="4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>2000</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H2" s="4">
+      <c r="F2" s="3">
         <v>2010</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="8" t="s">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>281</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="H3" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="G3" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2411,23 +2606,23 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>154</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2437,23 +2632,23 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
       </c>
       <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2463,23 +2658,23 @@
       <c r="C6" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>156</v>
       </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
       <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
         <v>156</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2489,23 +2684,23 @@
       <c r="C7" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>157</v>
       </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
       <c r="H7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" t="s">
         <v>231</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2515,23 +2710,23 @@
       <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>158</v>
       </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
       <c r="H8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
         <v>232</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2541,23 +2736,23 @@
       <c r="C9" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
       <c r="H9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" t="s">
         <v>233</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2567,23 +2762,23 @@
       <c r="C10" t="s">
         <v>185</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
       <c r="H10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" t="s">
         <v>234</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2593,23 +2788,23 @@
       <c r="C11" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" t="s">
         <v>235</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2619,23 +2814,23 @@
       <c r="C12" t="s">
         <v>187</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
       <c r="H12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" t="s">
         <v>236</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2645,23 +2840,23 @@
       <c r="C13" t="s">
         <v>188</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>163</v>
       </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
       <c r="H13" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" t="s">
         <v>237</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2671,23 +2866,23 @@
       <c r="C14" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="F14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
       <c r="H14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" t="s">
         <v>238</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2697,23 +2892,23 @@
       <c r="C15" t="s">
         <v>190</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>165</v>
       </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
       <c r="H15" t="s">
-        <v>112</v>
-      </c>
-      <c r="I15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" t="s">
         <v>239</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2723,23 +2918,23 @@
       <c r="C16" t="s">
         <v>191</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>166</v>
       </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
       <c r="H16" t="s">
-        <v>113</v>
-      </c>
-      <c r="I16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" t="s">
         <v>240</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2749,23 +2944,23 @@
       <c r="C17" t="s">
         <v>192</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
       <c r="H17" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" t="s">
         <v>241</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2775,23 +2970,23 @@
       <c r="C18" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="F18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
       <c r="H18" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J18" t="s">
         <v>242</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="I18" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2801,23 +2996,23 @@
       <c r="C19" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>169</v>
       </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
       <c r="H19" t="s">
-        <v>116</v>
-      </c>
-      <c r="I19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" t="s">
         <v>243</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2827,23 +3022,23 @@
       <c r="C20" t="s">
         <v>195</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
       <c r="H20" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" t="s">
-        <v>68</v>
-      </c>
-      <c r="J20" t="s">
         <v>244</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2853,23 +3048,23 @@
       <c r="C21" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>171</v>
       </c>
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
       <c r="H21" t="s">
-        <v>118</v>
-      </c>
-      <c r="I21" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" t="s">
         <v>245</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2879,23 +3074,23 @@
       <c r="C22" t="s">
         <v>197</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>172</v>
       </c>
+      <c r="F22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
       <c r="H22" t="s">
-        <v>119</v>
-      </c>
-      <c r="I22" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" t="s">
         <v>246</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2905,23 +3100,23 @@
       <c r="C23" t="s">
         <v>198</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
       <c r="H23" t="s">
-        <v>120</v>
-      </c>
-      <c r="I23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J23" t="s">
         <v>247</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="I23" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2931,23 +3126,23 @@
       <c r="C24" t="s">
         <v>199</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>174</v>
       </c>
+      <c r="F24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
       <c r="H24" t="s">
-        <v>121</v>
-      </c>
-      <c r="I24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" t="s">
         <v>248</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2957,23 +3152,23 @@
       <c r="C25" t="s">
         <v>200</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
       <c r="H25" t="s">
-        <v>122</v>
-      </c>
-      <c r="I25" t="s">
-        <v>73</v>
-      </c>
-      <c r="J25" t="s">
         <v>249</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2983,23 +3178,23 @@
       <c r="C26" t="s">
         <v>201</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>176</v>
       </c>
+      <c r="F26" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
       <c r="H26" t="s">
-        <v>123</v>
-      </c>
-      <c r="I26" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" t="s">
         <v>250</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3009,23 +3204,23 @@
       <c r="C27" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="F27" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
       <c r="H27" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" t="s">
-        <v>75</v>
-      </c>
-      <c r="J27" t="s">
         <v>251</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="I27" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3035,23 +3230,23 @@
       <c r="C28" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>178</v>
       </c>
+      <c r="F28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" t="s">
+        <v>76</v>
+      </c>
       <c r="H28" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" t="s">
         <v>252</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="I28" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3061,23 +3256,23 @@
       <c r="C29" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>179</v>
       </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" t="s">
+        <v>77</v>
+      </c>
       <c r="H29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I29" t="s">
-        <v>77</v>
-      </c>
-      <c r="J29" t="s">
         <v>253</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="I29" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3087,23 +3282,23 @@
       <c r="C30" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
       <c r="H30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I30" t="s">
-        <v>78</v>
-      </c>
-      <c r="J30" t="s">
         <v>254</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="I30" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3113,23 +3308,23 @@
       <c r="C31" t="s">
         <v>206</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>181</v>
       </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
       <c r="H31" t="s">
-        <v>128</v>
-      </c>
-      <c r="I31" t="s">
-        <v>79</v>
-      </c>
-      <c r="J31" t="s">
         <v>255</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="I31" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3139,17 +3334,17 @@
       <c r="C32" t="s">
         <v>207</v>
       </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" t="s">
+        <v>80</v>
+      </c>
       <c r="H32" t="s">
-        <v>129</v>
-      </c>
-      <c r="I32" t="s">
-        <v>80</v>
-      </c>
-      <c r="J32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3159,17 +3354,17 @@
       <c r="C33" t="s">
         <v>208</v>
       </c>
+      <c r="F33" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" t="s">
+        <v>81</v>
+      </c>
       <c r="H33" t="s">
-        <v>130</v>
-      </c>
-      <c r="I33" t="s">
-        <v>81</v>
-      </c>
-      <c r="J33" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3179,17 +3374,17 @@
       <c r="C34" t="s">
         <v>209</v>
       </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" t="s">
+        <v>82</v>
+      </c>
       <c r="H34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I34" t="s">
-        <v>82</v>
-      </c>
-      <c r="J34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3199,17 +3394,17 @@
       <c r="C35" t="s">
         <v>210</v>
       </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
       <c r="H35" t="s">
-        <v>132</v>
-      </c>
-      <c r="I35" t="s">
-        <v>83</v>
-      </c>
-      <c r="J35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3219,17 +3414,17 @@
       <c r="C36" t="s">
         <v>211</v>
       </c>
+      <c r="F36" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" t="s">
+        <v>84</v>
+      </c>
       <c r="H36" t="s">
-        <v>133</v>
-      </c>
-      <c r="I36" t="s">
-        <v>84</v>
-      </c>
-      <c r="J36" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3239,17 +3434,17 @@
       <c r="C37" t="s">
         <v>212</v>
       </c>
+      <c r="F37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
       <c r="H37" t="s">
-        <v>134</v>
-      </c>
-      <c r="I37" t="s">
-        <v>85</v>
-      </c>
-      <c r="J37" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3259,17 +3454,17 @@
       <c r="C38" t="s">
         <v>213</v>
       </c>
+      <c r="F38" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" t="s">
+        <v>86</v>
+      </c>
       <c r="H38" t="s">
-        <v>135</v>
-      </c>
-      <c r="I38" t="s">
-        <v>86</v>
-      </c>
-      <c r="J38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3279,17 +3474,17 @@
       <c r="C39" t="s">
         <v>214</v>
       </c>
+      <c r="F39" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" t="s">
+        <v>87</v>
+      </c>
       <c r="H39" t="s">
-        <v>136</v>
-      </c>
-      <c r="I39" t="s">
-        <v>87</v>
-      </c>
-      <c r="J39" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -3299,17 +3494,17 @@
       <c r="C40" t="s">
         <v>215</v>
       </c>
+      <c r="F40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
       <c r="H40" t="s">
-        <v>137</v>
-      </c>
-      <c r="I40" t="s">
-        <v>88</v>
-      </c>
-      <c r="J40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -3319,17 +3514,17 @@
       <c r="C41" t="s">
         <v>216</v>
       </c>
+      <c r="F41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" t="s">
+        <v>89</v>
+      </c>
       <c r="H41" t="s">
-        <v>138</v>
-      </c>
-      <c r="I41" t="s">
-        <v>89</v>
-      </c>
-      <c r="J41" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3339,17 +3534,17 @@
       <c r="C42" t="s">
         <v>217</v>
       </c>
+      <c r="F42" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
       <c r="H42" t="s">
-        <v>139</v>
-      </c>
-      <c r="I42" t="s">
-        <v>90</v>
-      </c>
-      <c r="J42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -3359,17 +3554,17 @@
       <c r="C43" t="s">
         <v>218</v>
       </c>
+      <c r="F43" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" t="s">
+        <v>91</v>
+      </c>
       <c r="H43" t="s">
-        <v>140</v>
-      </c>
-      <c r="I43" t="s">
-        <v>91</v>
-      </c>
-      <c r="J43" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -3379,17 +3574,17 @@
       <c r="C44" t="s">
         <v>219</v>
       </c>
+      <c r="F44" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" t="s">
+        <v>92</v>
+      </c>
       <c r="H44" t="s">
-        <v>141</v>
-      </c>
-      <c r="I44" t="s">
-        <v>92</v>
-      </c>
-      <c r="J44" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3399,17 +3594,17 @@
       <c r="C45" t="s">
         <v>220</v>
       </c>
+      <c r="F45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" t="s">
+        <v>93</v>
+      </c>
       <c r="H45" t="s">
-        <v>142</v>
-      </c>
-      <c r="I45" t="s">
-        <v>93</v>
-      </c>
-      <c r="J45" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -3419,17 +3614,17 @@
       <c r="C46" t="s">
         <v>221</v>
       </c>
+      <c r="F46" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" t="s">
+        <v>94</v>
+      </c>
       <c r="H46" t="s">
-        <v>143</v>
-      </c>
-      <c r="I46" t="s">
-        <v>94</v>
-      </c>
-      <c r="J46" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -3439,17 +3634,17 @@
       <c r="C47" t="s">
         <v>222</v>
       </c>
+      <c r="F47" t="s">
+        <v>144</v>
+      </c>
+      <c r="G47" t="s">
+        <v>95</v>
+      </c>
       <c r="H47" t="s">
-        <v>144</v>
-      </c>
-      <c r="I47" t="s">
-        <v>95</v>
-      </c>
-      <c r="J47" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -3459,17 +3654,17 @@
       <c r="C48" t="s">
         <v>223</v>
       </c>
+      <c r="F48" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" t="s">
+        <v>96</v>
+      </c>
       <c r="H48" t="s">
-        <v>145</v>
-      </c>
-      <c r="I48" t="s">
-        <v>96</v>
-      </c>
-      <c r="J48" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3479,17 +3674,17 @@
       <c r="C49" t="s">
         <v>224</v>
       </c>
+      <c r="F49" t="s">
+        <v>146</v>
+      </c>
+      <c r="G49" t="s">
+        <v>97</v>
+      </c>
       <c r="H49" t="s">
-        <v>146</v>
-      </c>
-      <c r="I49" t="s">
-        <v>97</v>
-      </c>
-      <c r="J49" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -3499,17 +3694,17 @@
       <c r="C50" t="s">
         <v>225</v>
       </c>
+      <c r="F50" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" t="s">
+        <v>98</v>
+      </c>
       <c r="H50" t="s">
-        <v>147</v>
-      </c>
-      <c r="I50" t="s">
-        <v>98</v>
-      </c>
-      <c r="J50" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -3519,17 +3714,17 @@
       <c r="C51" t="s">
         <v>226</v>
       </c>
+      <c r="F51" t="s">
+        <v>148</v>
+      </c>
+      <c r="G51" t="s">
+        <v>99</v>
+      </c>
       <c r="H51" t="s">
-        <v>148</v>
-      </c>
-      <c r="I51" t="s">
-        <v>99</v>
-      </c>
-      <c r="J51" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3539,17 +3734,17 @@
       <c r="C52" t="s">
         <v>227</v>
       </c>
+      <c r="F52" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" t="s">
+        <v>100</v>
+      </c>
       <c r="H52" t="s">
-        <v>149</v>
-      </c>
-      <c r="I52" t="s">
-        <v>100</v>
-      </c>
-      <c r="J52" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -3559,17 +3754,17 @@
       <c r="C53" t="s">
         <v>228</v>
       </c>
+      <c r="F53" t="s">
+        <v>150</v>
+      </c>
+      <c r="G53" t="s">
+        <v>101</v>
+      </c>
       <c r="H53" t="s">
-        <v>150</v>
-      </c>
-      <c r="I53" t="s">
-        <v>101</v>
-      </c>
-      <c r="J53" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3579,17 +3774,17 @@
       <c r="C54" t="s">
         <v>229</v>
       </c>
+      <c r="F54" t="s">
+        <v>151</v>
+      </c>
+      <c r="G54" t="s">
+        <v>102</v>
+      </c>
       <c r="H54" t="s">
-        <v>151</v>
-      </c>
-      <c r="I54" t="s">
-        <v>102</v>
-      </c>
-      <c r="J54" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -3599,13 +3794,13 @@
       <c r="C55" t="s">
         <v>230</v>
       </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+      <c r="G55" t="s">
+        <v>103</v>
+      </c>
       <c r="H55" t="s">
-        <v>152</v>
-      </c>
-      <c r="I55" t="s">
-        <v>103</v>
-      </c>
-      <c r="J55" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>